<commit_message>
added dish weights for half of the samples 20191029 to start AFDW process - samples in 75C for 12-24 hrs
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Phys.assays/Master_table.xlsx
+++ b/RAnalysis/Data/Phys.assays/Master_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\My_Projects\Inragenerational_thresholds_OA\RAnalysis\Data\Phys.assays\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{68CE9A1E-2916-4E11-A9B7-93675BBF9613}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A548F3F-8304-4143-A3BA-726617D21B30}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E167A34B-14A7-4443-B290-3C517896FDA9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{E167A34B-14A7-4443-B290-3C517896FDA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="115">
   <si>
     <t>Date.fixed</t>
   </si>
@@ -950,8 +950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2122E5-6B09-437B-B7A0-1511691F2B85}">
   <dimension ref="A1:U85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="I19" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1080,9 @@
       <c r="M2" s="4">
         <v>350</v>
       </c>
-      <c r="N2" s="4"/>
+      <c r="N2" s="4">
+        <v>0.45829999999999999</v>
+      </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
@@ -1126,7 +1128,9 @@
       <c r="M3" s="4">
         <v>350</v>
       </c>
-      <c r="N3" s="4"/>
+      <c r="N3" s="4">
+        <v>0.51529999999999998</v>
+      </c>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
@@ -1172,7 +1176,9 @@
       <c r="M4" s="4">
         <v>350</v>
       </c>
-      <c r="N4" s="4"/>
+      <c r="N4" s="4">
+        <v>0.5393</v>
+      </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
@@ -1218,7 +1224,9 @@
       <c r="M5" s="4">
         <v>350</v>
       </c>
-      <c r="N5" s="4"/>
+      <c r="N5" s="4">
+        <v>0.53539999999999999</v>
+      </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
@@ -1264,7 +1272,9 @@
       <c r="M6" s="4">
         <v>350</v>
       </c>
-      <c r="N6" s="4"/>
+      <c r="N6" s="4">
+        <v>0.51470000000000005</v>
+      </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
@@ -1310,7 +1320,9 @@
       <c r="M7" s="4">
         <v>350</v>
       </c>
-      <c r="N7" s="4"/>
+      <c r="N7" s="4">
+        <v>0.49969999999999998</v>
+      </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
@@ -1356,7 +1368,9 @@
       <c r="M8" s="4">
         <v>350</v>
       </c>
-      <c r="N8" s="4"/>
+      <c r="N8" s="4">
+        <v>0.45429999999999998</v>
+      </c>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
@@ -1402,7 +1416,9 @@
       <c r="M9" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="N9" s="7"/>
+      <c r="N9" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
@@ -1451,7 +1467,9 @@
       <c r="M10" s="4">
         <v>350</v>
       </c>
-      <c r="N10" s="4"/>
+      <c r="N10" s="4">
+        <v>0.46679999999999999</v>
+      </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
       <c r="Q10" s="4"/>
@@ -1497,7 +1515,9 @@
       <c r="M11" s="4">
         <v>350</v>
       </c>
-      <c r="N11" s="4"/>
+      <c r="N11" s="4">
+        <v>0.42430000000000001</v>
+      </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
       <c r="Q11" s="4"/>
@@ -1543,7 +1563,9 @@
       <c r="M12" s="4">
         <v>350</v>
       </c>
-      <c r="N12" s="4"/>
+      <c r="N12" s="4">
+        <v>0.50639999999999996</v>
+      </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="4"/>
@@ -1589,7 +1611,9 @@
       <c r="M13" s="4">
         <v>350</v>
       </c>
-      <c r="N13" s="4"/>
+      <c r="N13" s="4">
+        <v>0.47920000000000001</v>
+      </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
@@ -1635,7 +1659,9 @@
       <c r="M14" s="4">
         <v>350</v>
       </c>
-      <c r="N14" s="4"/>
+      <c r="N14" s="4">
+        <v>0.48499999999999999</v>
+      </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
@@ -1681,7 +1707,9 @@
       <c r="M15" s="4">
         <v>200</v>
       </c>
-      <c r="N15" s="4"/>
+      <c r="N15" s="4">
+        <v>0.59279999999999999</v>
+      </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
@@ -1727,7 +1755,9 @@
       <c r="M16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="N16" s="7"/>
+      <c r="N16" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
@@ -1776,7 +1806,9 @@
       <c r="M17" s="1">
         <v>100</v>
       </c>
-      <c r="N17" s="1"/>
+      <c r="N17" s="1">
+        <v>0.4662</v>
+      </c>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
@@ -1825,7 +1857,9 @@
       <c r="M18" s="1">
         <v>100</v>
       </c>
-      <c r="N18" s="1"/>
+      <c r="N18" s="1">
+        <v>0.35239999999999999</v>
+      </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -1874,7 +1908,9 @@
       <c r="M19" s="1">
         <v>50</v>
       </c>
-      <c r="N19" s="1"/>
+      <c r="N19" s="1">
+        <v>0.377</v>
+      </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -1923,7 +1959,9 @@
       <c r="M20" s="1">
         <v>100</v>
       </c>
-      <c r="N20" s="1"/>
+      <c r="N20" s="1">
+        <v>0.48120000000000002</v>
+      </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
@@ -1972,7 +2010,9 @@
       <c r="M21" s="1">
         <v>100</v>
       </c>
-      <c r="N21" s="1"/>
+      <c r="N21" s="1">
+        <v>0.38379999999999997</v>
+      </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
@@ -2021,7 +2061,9 @@
       <c r="M22" s="1">
         <v>100</v>
       </c>
-      <c r="N22" s="1"/>
+      <c r="N22" s="1">
+        <v>0.36749999999999999</v>
+      </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
@@ -2067,7 +2109,9 @@
       <c r="M23" s="1">
         <v>100</v>
       </c>
-      <c r="N23" s="1"/>
+      <c r="N23" s="1">
+        <v>0.43440000000000001</v>
+      </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
@@ -2113,7 +2157,9 @@
       <c r="M24" s="1">
         <v>100</v>
       </c>
-      <c r="N24" s="1"/>
+      <c r="N24" s="1">
+        <v>0.43369999999999997</v>
+      </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
@@ -2159,7 +2205,9 @@
       <c r="M25" s="1">
         <v>100</v>
       </c>
-      <c r="N25" s="1"/>
+      <c r="N25" s="1">
+        <v>0.55820000000000003</v>
+      </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -2205,7 +2253,9 @@
       <c r="M26" s="1">
         <v>100</v>
       </c>
-      <c r="N26" s="1"/>
+      <c r="N26" s="1">
+        <v>0.4718</v>
+      </c>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
@@ -2251,7 +2301,9 @@
       <c r="M27" s="1">
         <v>100</v>
       </c>
-      <c r="N27" s="1"/>
+      <c r="N27" s="1">
+        <v>0.55210000000000004</v>
+      </c>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
@@ -2297,7 +2349,9 @@
       <c r="M28" s="1">
         <v>100</v>
       </c>
-      <c r="N28" s="1"/>
+      <c r="N28" s="1">
+        <v>0.57709999999999995</v>
+      </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
@@ -2343,7 +2397,9 @@
       <c r="M29" s="1">
         <v>100</v>
       </c>
-      <c r="N29" s="1"/>
+      <c r="N29" s="1">
+        <v>0.4844</v>
+      </c>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
@@ -2389,7 +2445,9 @@
       <c r="M30" s="1">
         <v>100</v>
       </c>
-      <c r="N30" s="1"/>
+      <c r="N30" s="1">
+        <v>0.36370000000000002</v>
+      </c>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
@@ -2435,7 +2493,9 @@
       <c r="M31" s="1">
         <v>100</v>
       </c>
-      <c r="N31" s="1"/>
+      <c r="N31" s="1">
+        <v>0.43769999999999998</v>
+      </c>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
@@ -2481,7 +2541,9 @@
       <c r="M32" s="1">
         <v>100</v>
       </c>
-      <c r="N32" s="1"/>
+      <c r="N32" s="1">
+        <v>0.49299999999999999</v>
+      </c>
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -2527,7 +2589,9 @@
       <c r="M33" s="1">
         <v>100</v>
       </c>
-      <c r="N33" s="1"/>
+      <c r="N33" s="1">
+        <v>0.44819999999999999</v>
+      </c>
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
@@ -2573,7 +2637,9 @@
       <c r="M34" s="1">
         <v>100</v>
       </c>
-      <c r="N34" s="1"/>
+      <c r="N34" s="1">
+        <v>0.50580000000000003</v>
+      </c>
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
@@ -2619,7 +2685,9 @@
       <c r="M35" s="1">
         <v>100</v>
       </c>
-      <c r="N35" s="1"/>
+      <c r="N35" s="1">
+        <v>0.45600000000000002</v>
+      </c>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
@@ -2665,7 +2733,9 @@
       <c r="M36" s="1">
         <v>100</v>
       </c>
-      <c r="N36" s="1"/>
+      <c r="N36" s="1">
+        <v>0.40239999999999998</v>
+      </c>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
@@ -2711,7 +2781,9 @@
       <c r="M37" s="1">
         <v>100</v>
       </c>
-      <c r="N37" s="1"/>
+      <c r="N37" s="1">
+        <v>0.4012</v>
+      </c>
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
@@ -2757,7 +2829,9 @@
       <c r="M38" s="1">
         <v>100</v>
       </c>
-      <c r="N38" s="1"/>
+      <c r="N38" s="1">
+        <v>0.35420000000000001</v>
+      </c>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
@@ -2803,7 +2877,9 @@
       <c r="M39" s="1">
         <v>100</v>
       </c>
-      <c r="N39" s="1"/>
+      <c r="N39" s="1">
+        <v>0.47939999999999999</v>
+      </c>
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
@@ -2849,7 +2925,9 @@
       <c r="M40" s="1">
         <v>100</v>
       </c>
-      <c r="N40" s="1"/>
+      <c r="N40" s="1">
+        <v>0.43640000000000001</v>
+      </c>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
@@ -2895,7 +2973,9 @@
       <c r="M41" s="1">
         <v>100</v>
       </c>
-      <c r="N41" s="1"/>
+      <c r="N41" s="1">
+        <v>0.46489999999999998</v>
+      </c>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
@@ -2941,7 +3021,9 @@
       <c r="M42" s="1">
         <v>100</v>
       </c>
-      <c r="N42" s="1"/>
+      <c r="N42" s="1">
+        <v>0.47170000000000001</v>
+      </c>
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
@@ -2987,7 +3069,9 @@
       <c r="M43" s="1">
         <v>100</v>
       </c>
-      <c r="N43" s="1"/>
+      <c r="N43" s="1">
+        <v>0.43680000000000002</v>
+      </c>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
@@ -3033,7 +3117,9 @@
       <c r="M44" s="1">
         <v>100</v>
       </c>
-      <c r="N44" s="1"/>
+      <c r="N44" s="1">
+        <v>0.4612</v>
+      </c>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
@@ -3079,7 +3165,9 @@
       <c r="M45" s="1">
         <v>100</v>
       </c>
-      <c r="N45" s="1"/>
+      <c r="N45" s="1">
+        <v>0.50960000000000005</v>
+      </c>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
@@ -3125,7 +3213,9 @@
       <c r="M46" s="1">
         <v>100</v>
       </c>
-      <c r="N46" s="1"/>
+      <c r="N46" s="1">
+        <v>0.46460000000000001</v>
+      </c>
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>

</xml_diff>